<commit_message>
Uprev to 1.1 to support current parts availability Added solderpaste to USB connector through-pins
</commit_message>
<xml_diff>
--- a/Hardware/BackBoard Pogo Jig/BOM.xlsx
+++ b/Hardware/BackBoard Pogo Jig/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamster\Documents\Development\dc801\BM-Badge\Hardware\BackBoard Pogo Jig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE00B0F7-D9DA-44FC-98C0-55365E059BC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AE80B0-7EA4-4D15-9CC0-5AE41804204B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23010" yWindow="1080" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t>Ref Des</t>
   </si>
@@ -213,9 +213,6 @@
     <t>ED1012-ND</t>
   </si>
   <si>
-    <t>C1,C15,C25</t>
-  </si>
-  <si>
     <t>C26</t>
   </si>
   <si>
@@ -235,6 +232,24 @@
   </si>
   <si>
     <t>Total Parts</t>
+  </si>
+  <si>
+    <t>C1,C14,C25</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>FT230XS</t>
+  </si>
+  <si>
+    <t>USB to serial</t>
+  </si>
+  <si>
+    <t>768-1135-1-ND</t>
+  </si>
+  <si>
+    <t>16SSOP</t>
   </si>
 </sst>
 </file>
@@ -584,7 +599,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +645,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -651,7 +666,7 @@
         <v>1.78E-2</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I16" si="0">G2*H2</f>
+        <f t="shared" ref="I2:I18" si="0">G2*H2</f>
         <v>5.3400000000000003E-2</v>
       </c>
     </row>
@@ -684,7 +699,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
@@ -738,7 +753,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -876,7 +891,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -951,7 +966,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1032,7 +1047,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
@@ -1046,24 +1061,61 @@
       <c r="G17">
         <v>19</v>
       </c>
+      <c r="H17">
+        <v>0.39</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>7.41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>2.04</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>2.04</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G21">
         <f>SUM(G4:G19)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I21">
         <f>SUM(I4:I19)</f>
-        <v>9.0198200000000028</v>
+        <v>18.469820000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>